<commit_message>
calorimetry : input and output consistency : done
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.3.ampoule.bad.no.opt/data.xlsx
+++ b/input/calorimetry/ds.3.ampoule.bad.no.opt/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
@@ -653,7 +653,7 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -890,10 +890,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -925,6 +925,8 @@
         <v>-2.96</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>